<commit_message>
Plot all Stage 2 figures
Includes minor debugging of cleanup code to deal with inconsistencies in data reporting across Stages 1 and 2
</commit_message>
<xml_diff>
--- a/00_raw_data/CM_Stage1_submitted-2023-01-03.xlsx
+++ b/00_raw_data/CM_Stage1_submitted-2023-01-03.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836C2025-55C0-D846-B365-325B7766A8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E711BA-1356-D345-9FCA-E5245E7B43E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="19560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1080" windowWidth="34560" windowHeight="19560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -817,7 +817,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +895,15 @@
       <sz val="10"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -984,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1145,6 +1154,9 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,7 +1759,7 @@
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E12" sqref="E12"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1792,7 +1804,7 @@
       <c r="F1" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="62" t="s">
         <v>234</v>
       </c>
       <c r="H1" s="7" t="s">

</xml_diff>